<commit_message>
Basic the sistem is finished
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,69 +495,78 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Elias Gabriel Marinho de Oliveira</t>
+          <t>Eliseu Miguel</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Segunda Travessa Jose Coelho</t>
+          <t>Itabuna</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>Ba</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Santo Antonio</t>
+          <t>73 991920444</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Itabuna</t>
+          <t>10/06/2002</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>mguelmarinho@hotmail.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>45602028</t>
+          <t>3900</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>73 991920444</t>
+          <t>Interessado</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>eliasmarinho@hotmail.com</t>
+          <t>Apartamento</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>Imóvel Próprio</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Promissor</t>
+          <t>36 meses</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Apartamento</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
+          <t>R$250.000,00</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Financimaneto</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -565,242 +574,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Katiusscia Marinho de Oliveira</t>
+          <t>Elias Gabriel Marinho de Oliveira</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2° Travessa Jose Coelho</t>
+          <t>Itabuna</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>Ba</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Santo Antonio</t>
+          <t>73 991726631</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Itabuna</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ba</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>45602028</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>73 991203104</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>ktiusscia@hotmail.com</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Leads Novo</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Terreno</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Eliseu Miguel Marinho de Oliveira</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Rua Jose Coelho</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>152</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Santo Antonio</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Itabuna</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ba</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>45602018</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>73 991920444</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>mguelmarinho@hotmail.com</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>3800</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Promissor</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Apartamento</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Valor aproximado do imvóvel: 250k</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Iati Gomes Monteiro</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Rua K</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1649</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Cidadelle</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Itabuna</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Ba</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>iatigm@hotmail.com</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>30000</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Interessado</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Galpão</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Lair Sousa Alves</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Rua Manoel Bandeira</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>145</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Banco Raso</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Itabuna </t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Ba</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>4000</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Leads Novo</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+          <t>29/07/1998</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>